<commit_message>
Data Layers and Objects
</commit_message>
<xml_diff>
--- a/chicksComplete.xlsx
+++ b/chicksComplete.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Image processed</t>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -586,17 +586,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>falda</t>
+          <t>profile-cowboyshot</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>watercolor</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>woman</t>
+          <t>girl</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -610,17 +610,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3quarters-mediumshotdown</t>
+          <t>portrait-of-a-young-girl-happy-and-smiling-looking-pleased-and-successful-H9G13J</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>stan lee comic</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>woman</t>
+          <t>girl</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
@@ -634,12 +634,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3quarters-mediumshotdown</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>dibujo</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -658,12 +658,12 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>DonnaTroy</t>
+          <t>front-mediumshot5</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>porn toon</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -694,17 +694,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>images</t>
+          <t>rave</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>alphonse mucha style</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>tranny</t>
+          <t>woman</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -718,23 +718,23 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>maiteperronir</t>
+          <t>a10</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>manga</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>girl</t>
+          <t>woman</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
-          <t>concurrent.futures._base.CancelledError</t>
+          <t>Image processed</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -742,12 +742,12 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>c207bb40d43e6fe4_netimgAF5n1Z</t>
+          <t>portrait-of-a-young-girl-happy-and-smiling-looking-pleased-and-successful-H9G13J</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>masterpiece</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -758,7 +758,7 @@
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
-          <t>concurrent.futures._base.CancelledError</t>
+          <t>Image processed</t>
         </is>
       </c>
       <c r="V3" t="n">
@@ -771,12 +771,12 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>dibujo</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>tranny</t>
+          <t>girl</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr"/>
@@ -794,7 +794,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>concurrent.futures._base.CancelledError</t>
+          <t>Image processed</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -802,37 +802,91 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>sexy</t>
+          <t>wow</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>alphonse mucha style</t>
+          <t>Anime</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>girl</t>
+          <t>woman</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>3quarters-fullshot</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>4</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>AgachaCheer</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -846,29 +900,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>front-mediumshot3</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>AzuletteCosplay</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshot</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -882,29 +1008,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>rave</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>front-mediumshotdown2</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>front-mediumshot6</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>BlueDress</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -918,29 +1116,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>skirt</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Pose_Dress_Hands_Glance_Beautiful_590856_746x1024</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>4</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -954,29 +1224,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>cheer</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CaroGil</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>profile-cowboyshot</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>4</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>front-mediumshot</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -990,29 +1332,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>front-mediumshotdown1</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>c207bb40d43e6fe4_netimgAF5n1Z</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>4</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>blonde_boobs</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1026,29 +1440,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>maiteperronir</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>BelindaPop</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>4</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>images</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -1062,29 +1548,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nude-squat-9</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>AgachaCheer</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>EstefaníaMontaño</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>4</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>1520115753422</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1098,29 +1656,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshotdown</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>CaroGil</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>superhero</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>4</v>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshotdown</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -1134,29 +1764,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshotdown</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>front-mediumshot</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>front-mediumshot5</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>4</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>dancing</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -1170,29 +1872,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>tornivela</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>fb</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>front-mediumshotdown1</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>4</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1206,29 +1980,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>front-mediumshot7</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>skirt</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>front-medium-arms</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>4</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshot</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -1242,29 +2088,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>front-mediumshotdown</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>middle-age-senior-woman-curly</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>front-mediumshot10</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>4</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>boobs</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -1278,29 +2196,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>2</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>DonnaTroy</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>4</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>tornivela</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1314,29 +2304,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>portrait-of-a-young-girl-happy-and-smiling-looking-pleased-and-successful-H9G13J</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>RearView</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>tornivela</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>4</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshot1</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -1350,29 +2412,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshot</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>front-mediumshot3</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>4</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>c61308b17ab22b1354cc58def49d7ecd</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z19" t="inlineStr"/>
     </row>
     <row r="20">
@@ -1386,29 +2520,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>2</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>falda</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>DamarizGonzalez</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>4</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>BlueDress</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -1422,29 +2628,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>boobs</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>2</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>IMG_8794</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V21" t="n">
+        <v>4</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -1458,29 +2736,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>2</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>nude-squat-9</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>front-mediumshot6</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>4</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>c61308b17ab22b1354cc58def49d7ecd</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>girl</t>
+        </is>
+      </c>
       <c r="Z22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -1494,29 +2844,101 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>front-mediumshot9</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>2</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>front-mediumshot8</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>3quarters-mediumshot3</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>tranny</t>
+        </is>
+      </c>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V23" t="n">
+        <v>4</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>front-mediumshot1</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="Z23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -1530,11 +2952,29 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>front-mediumshot1</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Anime</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>woman</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>

</xml_diff>